<commit_message>
absolute % calculations fixed 2
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -1937,7 +1937,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1950,6 +1950,12 @@
       <sz val="11"/>
       <color rgb="FFc00000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -2023,40 +2029,40 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="22" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2471,7 +2477,7 @@
         <v>45652.735972222225</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="25.2">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -13123,7 +13129,7 @@
         <v>0</v>
       </c>
       <c r="E285" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F285" s="9">
         <v>0</v>

</xml_diff>